<commit_message>
Error with second moment fixed
</commit_message>
<xml_diff>
--- a/Data/Queue Data.xlsx
+++ b/Data/Queue Data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="18">
   <si>
     <t>min</t>
   </si>
@@ -33,21 +33,6 @@
   </si>
   <si>
     <t>max</t>
-  </si>
-  <si>
-    <t>5r/s</t>
-  </si>
-  <si>
-    <t>10r/s</t>
-  </si>
-  <si>
-    <t>20r/s</t>
-  </si>
-  <si>
-    <t>40r/s</t>
-  </si>
-  <si>
-    <t>100r/s</t>
   </si>
   <si>
     <t>Spec : Server computer : I7 7700k@5Ghz,8Go DDR4 Ram@2433Mhz,Ethernet connection between the two computers</t>
@@ -80,22 +65,19 @@
     <t>Matrices were size 40 and content was randomized real between 0 and 250</t>
   </si>
   <si>
-    <t>22,89ms</t>
+    <t>Rho</t>
   </si>
   <si>
-    <t>541,64ms</t>
+    <t>s</t>
   </si>
   <si>
-    <t>483,72ms</t>
+    <t>E[R]</t>
   </si>
   <si>
-    <t>21,45ms</t>
+    <t>E[R] = E[S] + Lambda*E[S²]/2*(1-Rho)</t>
   </si>
   <si>
-    <t>18,11ms</t>
-  </si>
-  <si>
-    <t>339,87ms</t>
+    <t>UNSTABLE</t>
   </si>
 </sst>
 </file>
@@ -139,13 +121,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -331,27 +310,28 @@
             </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>Sheet1!$E$8:$I$8</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>5r/s</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10r/s</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20r/s</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40r/s</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100r/s</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -466,27 +446,28 @@
             </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>Sheet1!$E$8:$I$8</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>5r/s</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10r/s</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20r/s</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40r/s</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100r/s</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -601,27 +582,28 @@
             </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>Sheet1!$E$8:$I$8</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>5r/s</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10r/s</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20r/s</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40r/s</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100r/s</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -1130,27 +1112,28 @@
             </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>Sheet1!$E$14:$I$14</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>5r/s</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10r/s</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20r/s</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40r/s</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100r/s</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -1265,27 +1248,28 @@
             </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>Sheet1!$E$14:$I$14</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>5r/s</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10r/s</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20r/s</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40r/s</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100r/s</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -1400,27 +1384,28 @@
             </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>Sheet1!$E$14:$I$14</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>5r/s</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10r/s</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20r/s</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40r/s</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100r/s</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -1934,27 +1919,28 @@
             </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>Sheet1!$E$20:$I$20</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>5r/s</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10r/s</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20r/s</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40r/s</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100r/s</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -2069,27 +2055,28 @@
             </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>Sheet1!$E$20:$I$20</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>5r/s</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10r/s</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20r/s</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40r/s</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100r/s</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -2204,27 +2191,28 @@
             </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>Sheet1!$E$20:$I$20</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>5r/s</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10r/s</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20r/s</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40r/s</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100r/s</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -4278,15 +4266,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>4762</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>595312</xdr:colOff>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -5184,58 +5172,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D3:L23"/>
+  <dimension ref="A3:M45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="17.5703125" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="4" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D5" t="s">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
         <v>8</v>
       </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="F8">
+        <v>10</v>
+      </c>
+      <c r="G8">
+        <v>20</v>
+      </c>
+      <c r="H8">
+        <v>40</v>
+      </c>
+      <c r="I8">
+        <v>100</v>
+      </c>
     </row>
-    <row r="6" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" t="s">
-        <v>3</v>
-      </c>
-      <c r="F8" t="s">
-        <v>4</v>
-      </c>
-      <c r="G8" t="s">
-        <v>5</v>
-      </c>
-      <c r="H8" t="s">
-        <v>6</v>
-      </c>
-      <c r="I8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f>(E8*E8*L11)/2*(1-E12)</f>
+        <v>5.848201124999999E-3</v>
+      </c>
       <c r="D9" t="s">
         <v>0</v>
       </c>
@@ -5255,13 +5248,13 @@
         <v>14</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="10" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
         <v>1</v>
       </c>
@@ -5280,14 +5273,10 @@
       <c r="I10">
         <v>38.89</v>
       </c>
-      <c r="K10" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
         <v>2</v>
       </c>
@@ -5306,30 +5295,86 @@
       <c r="I11">
         <v>318.27999999999997</v>
       </c>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
+      <c r="K11" s="2">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="L11" s="2">
+        <v>5.2568099999999996E-4</v>
+      </c>
+      <c r="M11" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="14" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12">
+        <f>E8*K11</f>
+        <v>0.10999999999999999</v>
+      </c>
+      <c r="F12">
+        <f>F8*K11</f>
+        <v>0.21999999999999997</v>
+      </c>
+      <c r="G12">
+        <f>G8*K11</f>
+        <v>0.43999999999999995</v>
+      </c>
+      <c r="H12">
+        <f>H8*K11</f>
+        <v>0.87999999999999989</v>
+      </c>
+      <c r="I12">
+        <f>I8*K11</f>
+        <v>2.1999999999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13">
+        <f>K11+(E8*L11)/(2*(1-E12))</f>
+        <v>2.347663202247191E-2</v>
+      </c>
+      <c r="F13">
+        <f>K11+(F8*L11)/(2*(1-F12))</f>
+        <v>2.536975E-2</v>
+      </c>
+      <c r="G13">
+        <f>K11+(G8*L11)/(2*(1-G12))</f>
+        <v>3.1387160714285711E-2</v>
+      </c>
+      <c r="H13">
+        <f>K11+(H8*L11)/(2*(1-H12))</f>
+        <v>0.10961349999999992</v>
+      </c>
+      <c r="I13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" t="s">
-        <v>3</v>
-      </c>
-      <c r="F14" t="s">
         <v>4</v>
       </c>
-      <c r="G14" t="s">
+      <c r="E14">
         <v>5</v>
       </c>
-      <c r="H14" t="s">
-        <v>6</v>
-      </c>
-      <c r="I14" t="s">
-        <v>7</v>
+      <c r="F14">
+        <v>10</v>
+      </c>
+      <c r="G14">
+        <v>20</v>
+      </c>
+      <c r="H14">
+        <v>40</v>
+      </c>
+      <c r="I14">
+        <v>100</v>
       </c>
     </row>
-    <row r="15" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
         <v>0</v>
       </c>
@@ -5349,13 +5394,13 @@
         <v>16</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="16" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
         <v>1</v>
       </c>
@@ -5374,14 +5419,10 @@
       <c r="I16">
         <v>40.299999999999997</v>
       </c>
-      <c r="K16" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="L16" s="3" t="s">
-        <v>20</v>
-      </c>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
         <v>2</v>
       </c>
@@ -5400,35 +5441,89 @@
       <c r="I17">
         <v>306.33999999999997</v>
       </c>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
+      <c r="K17" s="2">
+        <v>2.137E-2</v>
+      </c>
+      <c r="L17" s="2">
+        <v>4.704E-4</v>
+      </c>
+      <c r="M17" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="18" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18">
+        <f>E14*K17</f>
+        <v>0.10685</v>
+      </c>
+      <c r="F18">
+        <f>F14*K17</f>
+        <v>0.2137</v>
+      </c>
+      <c r="G18">
+        <f>G14*K17</f>
+        <v>0.4274</v>
+      </c>
+      <c r="H18">
+        <f>H14*K17</f>
+        <v>0.8548</v>
+      </c>
+      <c r="I18">
+        <f>I14*K17</f>
+        <v>2.137</v>
+      </c>
       <c r="L18" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="20" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19">
+        <f>K17+(E14*L17)/(2*(1-E18))</f>
+        <v>2.2686688126294575E-2</v>
+      </c>
+      <c r="F19">
+        <f>K17+(F14*L17)/(2*(1-F18))</f>
+        <v>2.436122472338802E-2</v>
+      </c>
+      <c r="G19">
+        <f>K17+(G14*L17)/(2*(1-G18))</f>
+        <v>2.9585158924205379E-2</v>
+      </c>
+      <c r="H19">
+        <f>K17+(H14*L17)/(2*(1-H18))</f>
+        <v>8.6163388429752061E-2</v>
+      </c>
+      <c r="I19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20">
+        <v>5</v>
+      </c>
+      <c r="F20">
         <v>10</v>
       </c>
-      <c r="E20" t="s">
-        <v>3</v>
-      </c>
-      <c r="F20" t="s">
-        <v>4</v>
-      </c>
-      <c r="G20" t="s">
-        <v>5</v>
-      </c>
-      <c r="H20" t="s">
-        <v>6</v>
-      </c>
-      <c r="I20" t="s">
-        <v>7</v>
+      <c r="G20">
+        <v>20</v>
+      </c>
+      <c r="H20">
+        <v>40</v>
+      </c>
+      <c r="I20">
+        <v>100</v>
       </c>
     </row>
-    <row r="21" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
         <v>0</v>
       </c>
@@ -5448,13 +5543,13 @@
         <v>18</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="22" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
         <v>1</v>
       </c>
@@ -5473,14 +5568,10 @@
       <c r="I22">
         <v>40.9</v>
       </c>
-      <c r="K22" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L22" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
     </row>
-    <row r="23" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
         <v>2</v>
       </c>
@@ -5499,8 +5590,72 @@
       <c r="I23">
         <v>309.39999999999998</v>
       </c>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
+      <c r="K23" s="2">
+        <v>2.4240000000000001E-2</v>
+      </c>
+      <c r="L23" s="2">
+        <v>6.5388000000000002E-4</v>
+      </c>
+      <c r="M23" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24">
+        <f>E20*K23</f>
+        <v>0.1212</v>
+      </c>
+      <c r="F24">
+        <f>F20*K23</f>
+        <v>0.2424</v>
+      </c>
+      <c r="G24">
+        <f>G20*K23</f>
+        <v>0.48480000000000001</v>
+      </c>
+      <c r="H24">
+        <f>H20*K23</f>
+        <v>0.96960000000000002</v>
+      </c>
+      <c r="I24">
+        <f>I20*K23</f>
+        <v>2.4239999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25">
+        <f>K23+(E20*L23)/(2*(1-E24))</f>
+        <v>2.6100150204824764E-2</v>
+      </c>
+      <c r="F25">
+        <f>K23+(F20*L23)/(2*(1-F24))</f>
+        <v>2.8555469904963042E-2</v>
+      </c>
+      <c r="G25">
+        <f>K23+(G20*L23)/(2*(1-G24))</f>
+        <v>3.6931770186335408E-2</v>
+      </c>
+      <c r="H25">
+        <f>K23+(H20*L23)/(2*(1-H24))</f>
+        <v>0.45442421052631604</v>
+      </c>
+      <c r="I25" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D45" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>